<commit_message>
Electricity Generated with multiple changes
</commit_message>
<xml_diff>
--- a/Region_LA_buildings.xlsx
+++ b/Region_LA_buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fintech Sandpit\ESG-entity-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D1C683-4C98-4086-B468-B3DF0ECCBBC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F484E8-8AB2-46DC-8390-BBC8B6AD40A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{86755C6B-ACE2-46DF-9925-663C115C7798}"/>
   </bookViews>
@@ -2639,7 +2639,7 @@
   <dimension ref="A1:AH369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2680,7 +2680,7 @@
     <col min="34" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>

</xml_diff>